<commit_message>
Fix header data mapping and display in DetalleObligaciones; update sidebar footer
</commit_message>
<xml_diff>
--- a/Archivo_v3.xlsx
+++ b/Archivo_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aure/Documents/Experimentación IA/AlertIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFECFCD-4D68-A14E-AB09-A4A3E77F1FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7699270D-DEA6-224C-8415-5EA00FFC241F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-17480" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -810,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -855,6 +855,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -862,21 +863,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1278,8 +1264,8 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1313,48 +1299,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
     </row>
     <row r="4" spans="1:29" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -1581,7 +1567,7 @@
       </c>
       <c r="R6" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" t="s">
@@ -1666,7 +1652,7 @@
       </c>
       <c r="R7" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" t="s">
@@ -1751,7 +1737,7 @@
       </c>
       <c r="R8" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" t="s">
@@ -1830,7 +1816,7 @@
       </c>
       <c r="R9" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" t="s">
@@ -1915,7 +1901,7 @@
       </c>
       <c r="R10" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" t="s">
@@ -1994,7 +1980,7 @@
       </c>
       <c r="R11" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" t="s">
@@ -2070,7 +2056,7 @@
       </c>
       <c r="R12" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" t="s">
@@ -2146,7 +2132,7 @@
       </c>
       <c r="R13" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" t="s">
@@ -2222,7 +2208,7 @@
       </c>
       <c r="R14" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" t="s">
@@ -2298,7 +2284,7 @@
       </c>
       <c r="R15" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" t="s">
@@ -2374,7 +2360,7 @@
       </c>
       <c r="R16" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" t="s">
@@ -2399,82 +2385,82 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="2:29" s="25" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
+    <row r="17" spans="2:29" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N17" s="21" t="s">
+      <c r="N17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="21" t="s">
+      <c r="O17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="8">
         <v>46044</v>
       </c>
-      <c r="Q17" s="23">
+      <c r="Q17" s="2">
         <v>46210</v>
       </c>
-      <c r="R17" s="24">
+      <c r="R17" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>2</v>
-      </c>
-      <c r="S17" s="21"/>
-      <c r="T17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" t="s">
         <v>193</v>
       </c>
-      <c r="U17" s="25" t="s">
+      <c r="U17" t="s">
         <v>194</v>
       </c>
-      <c r="V17" s="25" t="s">
+      <c r="V17" t="s">
         <v>209</v>
       </c>
-      <c r="Y17" s="26">
+      <c r="Y17" s="11">
         <v>46034</v>
       </c>
-      <c r="Z17" s="26">
+      <c r="Z17" s="11">
         <v>46037</v>
       </c>
-      <c r="AA17" s="27" t="s">
+      <c r="AA17" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="AB17" s="27" t="s">
+      <c r="AB17" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="AC17" s="27" t="s">
+      <c r="AC17" s="18" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2529,7 +2515,7 @@
       </c>
       <c r="R18" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="1"/>
       <c r="T18" t="s">
@@ -2605,7 +2591,7 @@
       </c>
       <c r="R19" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S19" s="1"/>
       <c r="T19" t="s">
@@ -2678,7 +2664,7 @@
       </c>
       <c r="R20" s="3">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="S20" s="1"/>
       <c r="T20" t="s">

</xml_diff>

<commit_message>
v3.0.2: Mejoras en detalle de obligación - Cabecera con datos del Excel, fecha límite desde columna P, estatus/subestatus, reglas de alertamiento desde columnas W-X-Y-Z, toggle de notificaciones
</commit_message>
<xml_diff>
--- a/Archivo_v3.xlsx
+++ b/Archivo_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aure/Documents/Experimentación IA/AlertIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7699270D-DEA6-224C-8415-5EA00FFC241F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EBDE1E-2A99-E341-879F-9ED485A8A842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-17480" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-17460" windowWidth="38400" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="214">
   <si>
     <t>Matriz de obligaciones (plantilla con lógica de fechas)</t>
   </si>
@@ -810,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -836,9 +836,6 @@
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
@@ -1263,9 +1260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="150" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1299,135 +1296,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
     </row>
     <row r="4" spans="1:29" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="S4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="U4" s="17" t="s">
+      <c r="U4" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="V4" s="17" t="s">
+      <c r="V4" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="W4" s="17" t="s">
+      <c r="W4" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="X4" s="17" t="s">
+      <c r="X4" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="Y4" s="17" t="s">
+      <c r="Y4" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="Z4" s="17" t="s">
+      <c r="Z4" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="AA4" s="17" t="s">
+      <c r="AA4" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="AB4" s="17" t="s">
+      <c r="AB4" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="AC4" s="17" t="s">
+      <c r="AC4" s="16" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1477,15 +1474,15 @@
       <c r="O5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="10" t="s">
-        <v>31</v>
+      <c r="P5" s="2">
+        <v>46235</v>
       </c>
       <c r="Q5" s="2">
         <v>46112</v>
       </c>
-      <c r="R5" s="9" t="e">
+      <c r="R5" s="9">
         <f ca="1">tbl_obligaciones[[#This Row],[Fecha límite de entrega]]-TODAY()</f>
-        <v>#VALUE!</v>
+        <v>192</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" t="s">
@@ -1497,19 +1494,19 @@
       <c r="V5" t="s">
         <v>174</v>
       </c>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11">
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10">
         <v>46106</v>
       </c>
-      <c r="AA5" s="12" t="s">
+      <c r="AA5" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AB5" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AC5" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1579,25 +1576,25 @@
       <c r="V6" t="s">
         <v>175</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6" s="10">
         <v>46143</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6" s="10">
         <v>46174</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6" s="10">
         <v>46204</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6" s="10">
         <v>46228</v>
       </c>
-      <c r="AA6" s="12" t="s">
+      <c r="AA6" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB6" s="12" t="s">
+      <c r="AB6" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC6" s="12" t="s">
+      <c r="AC6" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1664,25 +1661,25 @@
       <c r="V7" t="s">
         <v>176</v>
       </c>
-      <c r="W7" s="11">
+      <c r="W7" s="10">
         <v>46054</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="10">
         <v>46082</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="Y7" s="10">
         <v>46113</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="10">
         <v>46132</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AA7" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB7" s="12" t="s">
+      <c r="AB7" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AC7" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1749,19 +1746,19 @@
       <c r="V8" t="s">
         <v>177</v>
       </c>
-      <c r="Y8" s="11">
+      <c r="Y8" s="10">
         <v>46082</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="Z8" s="10">
         <v>46113</v>
       </c>
-      <c r="AA8" s="12" t="s">
+      <c r="AA8" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB8" s="12" t="s">
+      <c r="AB8" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC8" s="12" t="s">
+      <c r="AC8" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1828,25 +1825,25 @@
       <c r="V9" t="s">
         <v>178</v>
       </c>
-      <c r="W9" s="11">
+      <c r="W9" s="10">
         <v>46037</v>
       </c>
-      <c r="X9" s="11">
+      <c r="X9" s="10">
         <v>46082</v>
       </c>
-      <c r="Y9" s="11">
+      <c r="Y9" s="10">
         <v>46096</v>
       </c>
-      <c r="Z9" s="11">
+      <c r="Z9" s="10">
         <v>46101</v>
       </c>
-      <c r="AA9" s="12" t="s">
+      <c r="AA9" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB9" s="12" t="s">
+      <c r="AB9" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC9" s="12" t="s">
+      <c r="AC9" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1913,19 +1910,19 @@
       <c r="V10" t="s">
         <v>179</v>
       </c>
-      <c r="Y10" s="11">
+      <c r="Y10" s="10">
         <v>46051</v>
       </c>
-      <c r="Z10" s="11">
+      <c r="Z10" s="10">
         <v>46073</v>
       </c>
-      <c r="AA10" s="12" t="s">
+      <c r="AA10" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB10" s="12" t="s">
+      <c r="AB10" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC10" s="12" t="s">
+      <c r="AC10" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1992,16 +1989,16 @@
       <c r="V11" t="s">
         <v>180</v>
       </c>
-      <c r="X11" s="11">
+      <c r="X11" s="10">
         <v>46034</v>
       </c>
-      <c r="AA11" s="12" t="s">
+      <c r="AA11" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB11" s="12" t="s">
+      <c r="AB11" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC11" s="12" t="s">
+      <c r="AC11" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2068,16 +2065,16 @@
       <c r="V12" t="s">
         <v>181</v>
       </c>
-      <c r="W12" s="11">
+      <c r="W12" s="10">
         <v>46054</v>
       </c>
-      <c r="AA12" s="12" t="s">
+      <c r="AA12" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB12" s="12" t="s">
+      <c r="AB12" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC12" s="12" t="s">
+      <c r="AC12" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2144,16 +2141,16 @@
       <c r="V13" t="s">
         <v>182</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="Y13" s="10">
         <v>46037</v>
       </c>
-      <c r="AA13" s="12" t="s">
+      <c r="AA13" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB13" s="12" t="s">
+      <c r="AB13" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC13" s="12" t="s">
+      <c r="AC13" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2220,16 +2217,16 @@
       <c r="V14" t="s">
         <v>183</v>
       </c>
-      <c r="Z14" s="11">
+      <c r="Z14" s="10">
         <v>46047</v>
       </c>
-      <c r="AA14" s="12" t="s">
+      <c r="AA14" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB14" s="12" t="s">
+      <c r="AB14" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC14" s="12" t="s">
+      <c r="AC14" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2296,16 +2293,16 @@
       <c r="V15" t="s">
         <v>184</v>
       </c>
-      <c r="W15" s="11">
+      <c r="W15" s="10">
         <v>46054</v>
       </c>
-      <c r="AA15" s="12" t="s">
+      <c r="AA15" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB15" s="12" t="s">
+      <c r="AB15" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC15" s="12" t="s">
+      <c r="AC15" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2372,16 +2369,16 @@
       <c r="V16" t="s">
         <v>185</v>
       </c>
-      <c r="Y16" s="11">
+      <c r="Y16" s="10">
         <v>46042</v>
       </c>
-      <c r="AA16" s="12" t="s">
+      <c r="AA16" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB16" s="12" t="s">
+      <c r="AB16" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC16" s="12" t="s">
+      <c r="AC16" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2448,19 +2445,19 @@
       <c r="V17" t="s">
         <v>209</v>
       </c>
-      <c r="Y17" s="11">
+      <c r="Y17" s="10">
         <v>46034</v>
       </c>
-      <c r="Z17" s="11">
+      <c r="Z17" s="10">
         <v>46037</v>
       </c>
-      <c r="AA17" s="18" t="s">
+      <c r="AA17" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="AB17" s="18" t="s">
+      <c r="AB17" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="AC17" s="18" t="s">
+      <c r="AC17" s="17" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2527,16 +2524,16 @@
       <c r="V18" t="s">
         <v>186</v>
       </c>
-      <c r="Z18" s="11">
+      <c r="Z18" s="10">
         <v>46078</v>
       </c>
-      <c r="AA18" s="12" t="s">
+      <c r="AA18" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB18" s="12" t="s">
+      <c r="AB18" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC18" s="12" t="s">
+      <c r="AC18" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2603,13 +2600,13 @@
       <c r="V19" t="s">
         <v>187</v>
       </c>
-      <c r="AA19" s="12" t="s">
+      <c r="AA19" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB19" s="12" t="s">
+      <c r="AB19" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC19" s="12" t="s">
+      <c r="AC19" s="11" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2676,13 +2673,13 @@
       <c r="V20" t="s">
         <v>188</v>
       </c>
-      <c r="AA20" s="12" t="s">
+      <c r="AA20" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="AB20" s="12" t="s">
+      <c r="AB20" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="AC20" s="12" t="s">
+      <c r="AC20" s="11" t="s">
         <v>207</v>
       </c>
     </row>

</xml_diff>